<commit_message>
change format soal excel
</commit_message>
<xml_diff>
--- a/public/userfile/excel/soal.xlsx
+++ b/public/userfile/excel/soal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Installation\laragon\www\e-learning-bppt\public\userfile\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76A5BF99-7CD0-40E7-9B72-1EA600A19F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F5E476-6FF1-49F4-A511-049F47A21FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8DDCFA83-62C7-4C1C-9532-3D0CC4786D5C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>TIPE</t>
   </si>
@@ -39,9 +39,6 @@
     <t>PERTANYAAN</t>
   </si>
   <si>
-    <t>PILIHAN</t>
-  </si>
-  <si>
     <t>multiple_choice</t>
   </si>
   <si>
@@ -57,15 +54,9 @@
     <t>pertanyaan multiple choice</t>
   </si>
   <si>
-    <t>pilihna1 (jawaban); pilihan 2; pilihan 3; pilihan 4</t>
-  </si>
-  <si>
     <t>pertanyaan exact</t>
   </si>
   <si>
-    <t>jawaban 1; jawaban 2; jawaban 3</t>
-  </si>
-  <si>
     <t>pertanyaan essay</t>
   </si>
   <si>
@@ -73,6 +64,51 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>PILIHAN 1</t>
+  </si>
+  <si>
+    <t>PILIHAN 2</t>
+  </si>
+  <si>
+    <t>PILIHAN 3</t>
+  </si>
+  <si>
+    <t>PILIHAN 4</t>
+  </si>
+  <si>
+    <t>PILIHAN 5</t>
+  </si>
+  <si>
+    <t>pilihan 1 (jawaban)</t>
+  </si>
+  <si>
+    <t>pilihan 2</t>
+  </si>
+  <si>
+    <t>pilihan 3</t>
+  </si>
+  <si>
+    <t>pilihan 4</t>
+  </si>
+  <si>
+    <t>pilihan 5</t>
+  </si>
+  <si>
+    <t>jawaban 1</t>
+  </si>
+  <si>
+    <t>jawaban 2</t>
+  </si>
+  <si>
+    <t>jawaban 3</t>
+  </si>
+  <si>
+    <t>jiwaban 4</t>
+  </si>
+  <si>
+    <t>jawaban 5</t>
   </si>
 </sst>
 </file>
@@ -136,10 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -455,20 +492,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ED69D7-C275-420E-B79C-C714C67949E1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,50 +517,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>